<commit_message>
Changes of Order Processing for LOC and SD
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/AgentActivityChart.xlsx
+++ b/NetAgent/src/main/resources/AgentActivityChart.xlsx
@@ -180,10 +180,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>126365</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>155137</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>148475</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>215252</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -294,7 +294,7 @@
       </c>
       <c s="3" t="inlineStr" r="E7">
         <is>
-          <t xml:space="preserve">06/11/2022</t>
+          <t xml:space="preserve">06/14/2022</t>
         </is>
       </c>
       <c s="3" t="inlineStr" r="H7">
@@ -304,7 +304,7 @@
       </c>
       <c s="3" t="inlineStr" r="I7">
         <is>
-          <t xml:space="preserve">06/21/2022</t>
+          <t xml:space="preserve">06/24/2022</t>
         </is>
       </c>
     </row>
@@ -324,7 +324,7 @@
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="1.08332992125984" header="0.75" footer="0.75"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter alignWithMargins="0">
-    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;9 6/21/2022 12:42 AM &amp;C&amp;"Arial,Regular"&amp;9 Print User : automation &amp;R&amp;"Arial,Regular"&amp;9Page &amp;P of &amp;N </oddFooter>
+    <oddFooter>&amp;L&amp;"Arial,Regular"&amp;9 6/23/2022 10:51 PM &amp;C&amp;"Arial,Regular"&amp;9 Print User : automation &amp;R&amp;"Arial,Regular"&amp;9Page &amp;P of &amp;N </oddFooter>
   </headerFooter>
   <drawing r:id="rId7"/>
 </worksheet>

</xml_diff>